<commit_message>
merge con rama upload__finalizacion de merge
</commit_message>
<xml_diff>
--- a/out11.xlsx
+++ b/out11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G215"/>
+  <dimension ref="A1:G211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -486,12 +486,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>xe-0/0/0</t>
+          <t>xe-0/0/14</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -521,12 +521,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>xe-0/0/26</t>
+          <t>xe-0/0/15</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -556,12 +556,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>xe-0/0/27</t>
+          <t>xe-0/0/16</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -591,12 +591,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>xe-0/0/28</t>
+          <t>xe-0/0/17</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -626,12 +626,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>xe-0/0/29</t>
+          <t>xe-0/0/18</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -661,12 +661,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>xe-0/0/30</t>
+          <t>xe-0/0/19</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -696,12 +696,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>xe-0/0/31</t>
+          <t>xe-0/0/20</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -731,12 +731,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>xe-0/0/32</t>
+          <t>xe-0/0/21</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -751,7 +751,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -766,12 +766,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>xe-0/0/33</t>
+          <t>xe-0/0/22</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -801,12 +801,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>xe-0/0/34</t>
+          <t>xe-0/0/23</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -836,12 +836,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>xe-0/0/35</t>
+          <t>xe-0/0/24</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -856,7 +856,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -871,12 +871,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>xe-0/0/36</t>
+          <t>xe-0/0/25</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -906,12 +906,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>xe-0/0/37</t>
+          <t>xe-0/0/26</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -926,7 +926,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -941,12 +941,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>xe-0/0/38</t>
+          <t>xe-0/0/27</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -976,12 +976,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>xe-0/0/39</t>
+          <t>xe-0/0/28</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -996,7 +996,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1011,12 +1011,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>xe-0/0/40</t>
+          <t>xe-0/0/29</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1046,12 +1046,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>xe-0/0/41</t>
+          <t>xe-0/0/30</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1081,12 +1081,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>xe-0/0/42</t>
+          <t>xe-0/0/31</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1116,12 +1116,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>xe-0/0/43</t>
+          <t>xe-0/0/32</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1151,12 +1151,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>xe-0/0/44</t>
+          <t>xe-0/0/33</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1186,12 +1186,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>xe-0/0/45</t>
+          <t>xe-0/0/34</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1221,12 +1221,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>xe-0/0/46</t>
+          <t>xe-0/0/36</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1256,12 +1256,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>xe-0/0/47</t>
+          <t>xe-0/0/37</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1291,12 +1291,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>xe-0/0/48</t>
+          <t>xe-0/0/38</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1326,12 +1326,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>xe-0/0/0</t>
+          <t>xe-0/0/39</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1361,12 +1361,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>xe-0/0/1</t>
+          <t>xe-0/0/40</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1396,12 +1396,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>xe-0/0/10</t>
+          <t>xe-0/0/41</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1431,12 +1431,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>xe-0/0/11</t>
+          <t>xe-0/0/42</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1451,12 +1451,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>11:0</t>
+          <t>14:0</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1466,12 +1466,12 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>xe-0/0/12</t>
+          <t>xe-0/0/43</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1486,12 +1486,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>11:1</t>
+          <t>14:1</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1501,12 +1501,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>xe-0/0/13</t>
+          <t>xe-0/0/44</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1521,12 +1521,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>12:0</t>
+          <t>15:0</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1536,12 +1536,12 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>xe-0/0/14</t>
+          <t>xe-0/0/45</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1556,12 +1556,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>12:1</t>
+          <t>15:1</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1571,12 +1571,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>xe-0/0/15</t>
+          <t>xe-0/0/46</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1591,12 +1591,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>13:0</t>
+          <t>16:0</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1606,12 +1606,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>xe-0/0/16</t>
+          <t>xe-0/0/47</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1626,12 +1626,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>13:1</t>
+          <t>16:1</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1641,12 +1641,12 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>xe-0/0/17</t>
+          <t>xe-0/0/48</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1661,12 +1661,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>14:0</t>
+          <t>17:0</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1674,21 +1674,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>xe-0/0/18</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1696,12 +1684,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>14:1</t>
+          <t>17:1</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1709,21 +1697,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>xe-0/0/19</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1731,12 +1707,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>15:0</t>
+          <t>18:0</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1744,21 +1720,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>xe-0/0/2</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1766,12 +1730,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>15:1</t>
+          <t>18:1</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1779,21 +1743,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>xe-0/0/20</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1801,7 +1753,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1814,21 +1766,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>xe-0/0/21</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1836,7 +1776,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1849,21 +1789,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>xe-0/0/22</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1871,7 +1799,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1884,21 +1812,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>xe-0/0/23</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1906,7 +1822,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1919,21 +1835,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>xe-0/0/24</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1941,7 +1845,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1954,21 +1858,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>xe-0/0/25</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1976,7 +1868,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1989,21 +1881,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>xe-0/0/26</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2011,7 +1891,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2024,21 +1904,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>xe-0/0/27</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2046,7 +1914,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2059,21 +1927,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>xe-0/0/28</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2081,7 +1937,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2094,21 +1950,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>xe-0/0/29</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2116,7 +1960,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2129,21 +1973,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>xe-0/0/3</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -2151,7 +1983,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2164,21 +1996,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>xe-0/0/30</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2186,7 +2006,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2199,21 +2019,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>xe-0/0/31</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -2221,7 +2029,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2234,21 +2042,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>xe-0/0/32</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2256,7 +2052,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2269,21 +2065,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>xe-0/0/33</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2291,7 +2075,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2304,21 +2088,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>xe-0/0/34</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2326,7 +2098,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2339,21 +2111,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>xe-0/0/35</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2361,7 +2121,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2374,21 +2134,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>xe-0/0/36</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2396,7 +2144,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2409,21 +2157,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>xe-0/0/37</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2431,7 +2167,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2444,21 +2180,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>xe-0/0/38</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2466,7 +2190,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2479,21 +2203,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>xe-0/0/39</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2501,7 +2213,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2514,21 +2226,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>xe-0/0/4</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2536,7 +2236,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2549,21 +2249,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>xe-0/0/40</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -2571,7 +2259,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2584,21 +2272,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>xe-0/0/41</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2606,7 +2282,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2619,21 +2295,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>xe-0/0/42</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2641,7 +2305,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2654,21 +2318,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>xe-0/0/43</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2676,7 +2328,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2689,21 +2341,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>xe-0/0/44</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2711,7 +2351,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2724,21 +2364,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>xe-0/0/45</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2746,7 +2374,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2759,21 +2387,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>xe-0/0/46</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2781,7 +2397,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2794,21 +2410,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>xe-0/0/47</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2816,7 +2420,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2829,21 +2433,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>xe-0/0/48</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2851,7 +2443,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2864,21 +2456,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>xe-0/0/5</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2886,7 +2466,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2899,21 +2479,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>xe-0/0/6</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2921,7 +2489,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2934,21 +2502,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>xe-0/0/7</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2956,7 +2512,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2969,21 +2525,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>xe-0/0/8</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2991,7 +2535,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3004,21 +2548,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>xe-0/0/9</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -3026,7 +2558,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3049,7 +2581,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3072,7 +2604,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3095,7 +2627,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3118,7 +2650,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3141,7 +2673,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3164,7 +2696,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3187,7 +2719,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3210,7 +2742,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3233,7 +2765,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3256,7 +2788,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3279,7 +2811,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3302,7 +2834,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3325,7 +2857,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3348,7 +2880,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3371,7 +2903,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3394,7 +2926,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3417,7 +2949,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3440,7 +2972,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3463,7 +2995,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3486,7 +3018,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3509,7 +3041,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3532,7 +3064,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3555,7 +3087,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3578,7 +3110,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3601,7 +3133,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3624,7 +3156,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3647,7 +3179,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3670,7 +3202,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3693,7 +3225,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3716,7 +3248,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3739,7 +3271,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3762,7 +3294,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3785,7 +3317,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3808,7 +3340,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3831,7 +3363,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3854,7 +3386,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3877,7 +3409,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3900,7 +3432,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3923,7 +3455,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3946,7 +3478,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3969,7 +3501,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3992,7 +3524,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -4015,7 +3547,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4038,7 +3570,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4061,7 +3593,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4084,7 +3616,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -4107,7 +3639,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -4130,7 +3662,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -4153,7 +3685,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4176,7 +3708,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -4199,12 +3731,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>5:0</t>
+          <t>60:0</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -4222,12 +3754,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>5:1</t>
+          <t>60:1</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -4245,12 +3777,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>60:0</t>
+          <t>61:0</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -4268,12 +3800,12 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>60:1</t>
+          <t>61:1</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -4291,12 +3823,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>61:0</t>
+          <t>62:0</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -4314,12 +3846,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>61:1</t>
+          <t>62:1</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -4337,12 +3869,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>62:0</t>
+          <t>63:0</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -4360,12 +3892,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>62:1</t>
+          <t>63:1</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -4383,12 +3915,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>63:0</t>
+          <t>64:0</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -4406,12 +3938,12 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>63:1</t>
+          <t>64:1</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4429,12 +3961,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>64:0</t>
+          <t>65:0</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4452,12 +3984,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>64:1</t>
+          <t>65:1</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4475,12 +4007,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>65:0</t>
+          <t>66:0</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4498,12 +4030,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>65:1</t>
+          <t>66:1</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4521,12 +4053,12 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>66:0</t>
+          <t>67:0</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4544,12 +4076,12 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>66:1</t>
+          <t>67:1</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4567,12 +4099,12 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>67:0</t>
+          <t>68:0</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4590,12 +4122,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>67:1</t>
+          <t>68:1</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4613,12 +4145,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>68:0</t>
+          <t>69:0</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4636,12 +4168,12 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>68:1</t>
+          <t>69:1</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4659,12 +4191,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>69:0</t>
+          <t>6:0</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4682,12 +4214,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>69:1</t>
+          <t>6:1</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4705,12 +4237,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>6:0</t>
+          <t>70:0</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4728,12 +4260,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>6:1</t>
+          <t>70:1</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -4751,12 +4283,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>70:0</t>
+          <t>71:0</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -4774,12 +4306,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>70:1</t>
+          <t>71:1</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -4797,12 +4329,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>71:0</t>
+          <t>72:0</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -4820,12 +4352,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>71:1</t>
+          <t>72:1</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -4843,12 +4375,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>72:0</t>
+          <t>73:0</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -4866,12 +4398,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>72:1</t>
+          <t>73:1</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -4889,12 +4421,12 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>73:0</t>
+          <t>74:0</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -4912,12 +4444,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>73:1</t>
+          <t>74:1</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -4935,12 +4467,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>74:0</t>
+          <t>75:0</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -4958,12 +4490,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>74:1</t>
+          <t>75:1</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -4981,12 +4513,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>75:0</t>
+          <t>76:0</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -5004,12 +4536,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>75:1</t>
+          <t>76:1</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -5027,12 +4559,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>76:0</t>
+          <t>77:0</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -5050,12 +4582,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>76:1</t>
+          <t>77:1</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -5073,12 +4605,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>77:0</t>
+          <t>78:0</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -5096,12 +4628,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>77:1</t>
+          <t>78:1</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -5119,12 +4651,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>78:0</t>
+          <t>79:0</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -5142,12 +4674,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>78:1</t>
+          <t>79:1</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -5165,12 +4697,12 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>79:0</t>
+          <t>80:0</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -5188,12 +4720,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>79:1</t>
+          <t>80:1</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -5211,12 +4743,12 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>7:0</t>
+          <t>81:0</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -5234,12 +4766,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>7:1</t>
+          <t>81:1</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -5257,12 +4789,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>80:0</t>
+          <t>82:0</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -5280,12 +4812,12 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>80:1</t>
+          <t>82:1</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -5303,12 +4835,12 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>81:0</t>
+          <t>83:0</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -5326,12 +4858,12 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>81:1</t>
+          <t>83:1</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -5349,12 +4881,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>82:0</t>
+          <t>84:0</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -5372,12 +4904,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>82:1</t>
+          <t>84:1</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
@@ -5395,12 +4927,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>83:0</t>
+          <t>85:0</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -5418,12 +4950,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>83:1</t>
+          <t>85:1</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -5441,12 +4973,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>84:0</t>
+          <t>86:0</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -5464,12 +4996,12 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>84:1</t>
+          <t>86:1</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -5487,12 +5019,12 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>85:0</t>
+          <t>87:0</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -5510,12 +5042,12 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>85:1</t>
+          <t>87:1</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
@@ -5533,12 +5065,12 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>86:0</t>
+          <t>88:0</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -5556,12 +5088,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>86:1</t>
+          <t>88:1</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -5579,12 +5111,12 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>87:0</t>
+          <t>89:0</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -5602,12 +5134,12 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>87:1</t>
+          <t>89:1</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -5625,12 +5157,12 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>88:0</t>
+          <t>8:0</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -5648,12 +5180,12 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>88:1</t>
+          <t>8:1</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -5671,12 +5203,12 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>89:0</t>
+          <t>90:0</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -5694,12 +5226,12 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>89:1</t>
+          <t>90:1</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -5717,12 +5249,12 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>8:0</t>
+          <t>91:0</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -5740,12 +5272,12 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>8:1</t>
+          <t>91:1</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -5763,12 +5295,12 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>90:0</t>
+          <t>92:0</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
@@ -5786,12 +5318,12 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>90:1</t>
+          <t>92:1</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
@@ -5809,12 +5341,12 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>91:0</t>
+          <t>93:0</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
@@ -5832,12 +5364,12 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>91:1</t>
+          <t>93:1</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
@@ -5855,12 +5387,12 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>92:0</t>
+          <t>94:0</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
@@ -5878,12 +5410,12 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>92:1</t>
+          <t>94:1</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
@@ -5901,12 +5433,12 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>93:0</t>
+          <t>95:0</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -5924,12 +5456,12 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>93:1</t>
+          <t>95:1</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
@@ -5947,12 +5479,12 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>94:0</t>
+          <t>96:0</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
@@ -5970,12 +5502,12 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>94:1</t>
+          <t>96:1</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
@@ -5993,12 +5525,12 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>95:0</t>
+          <t>97:0</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
@@ -6016,12 +5548,12 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>95:1</t>
+          <t>97:1</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
@@ -6039,12 +5571,12 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>96:0</t>
+          <t>98:0</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
@@ -6062,12 +5594,12 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>96:1</t>
+          <t>98:1</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
@@ -6085,12 +5617,12 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>97:0</t>
+          <t>99:0</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
@@ -6108,12 +5640,12 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>97:1</t>
+          <t>99:1</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
@@ -6131,12 +5663,12 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>98:0</t>
+          <t>9:0</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
@@ -6154,12 +5686,12 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>98:1</t>
+          <t>9:1</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
@@ -6170,98 +5702,6 @@
       <c r="E211" t="inlineStr"/>
       <c r="F211" t="inlineStr"/>
       <c r="G211" t="inlineStr"/>
-    </row>
-    <row r="212">
-      <c r="A212" s="1" t="n">
-        <v>210</v>
-      </c>
-      <c r="B212" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-06-COS</t>
-        </is>
-      </c>
-      <c r="C212" t="inlineStr">
-        <is>
-          <t>99:0</t>
-        </is>
-      </c>
-      <c r="D212" t="inlineStr">
-        <is>
-          <t>unlocked</t>
-        </is>
-      </c>
-      <c r="E212" t="inlineStr"/>
-      <c r="F212" t="inlineStr"/>
-      <c r="G212" t="inlineStr"/>
-    </row>
-    <row r="213">
-      <c r="A213" s="1" t="n">
-        <v>211</v>
-      </c>
-      <c r="B213" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-06-COS</t>
-        </is>
-      </c>
-      <c r="C213" t="inlineStr">
-        <is>
-          <t>99:1</t>
-        </is>
-      </c>
-      <c r="D213" t="inlineStr">
-        <is>
-          <t>unlocked</t>
-        </is>
-      </c>
-      <c r="E213" t="inlineStr"/>
-      <c r="F213" t="inlineStr"/>
-      <c r="G213" t="inlineStr"/>
-    </row>
-    <row r="214">
-      <c r="A214" s="1" t="n">
-        <v>212</v>
-      </c>
-      <c r="B214" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-06-COS</t>
-        </is>
-      </c>
-      <c r="C214" t="inlineStr">
-        <is>
-          <t>9:0</t>
-        </is>
-      </c>
-      <c r="D214" t="inlineStr">
-        <is>
-          <t>unlocked</t>
-        </is>
-      </c>
-      <c r="E214" t="inlineStr"/>
-      <c r="F214" t="inlineStr"/>
-      <c r="G214" t="inlineStr"/>
-    </row>
-    <row r="215">
-      <c r="A215" s="1" t="n">
-        <v>213</v>
-      </c>
-      <c r="B215" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-06-COS</t>
-        </is>
-      </c>
-      <c r="C215" t="inlineStr">
-        <is>
-          <t>9:1</t>
-        </is>
-      </c>
-      <c r="D215" t="inlineStr">
-        <is>
-          <t>unlocked</t>
-        </is>
-      </c>
-      <c r="E215" t="inlineStr"/>
-      <c r="F215" t="inlineStr"/>
-      <c r="G215" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Se separo la tabla despues en COS y DAAS
</commit_message>
<xml_diff>
--- a/out11.xlsx
+++ b/out11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G215"/>
+  <dimension ref="A1:G211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -486,12 +486,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>xe-0/0/0</t>
+          <t>xe-0/0/14</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -521,12 +521,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>xe-0/0/26</t>
+          <t>xe-0/0/15</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -556,12 +556,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>xe-0/0/27</t>
+          <t>xe-0/0/16</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -591,12 +591,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>xe-0/0/28</t>
+          <t>xe-0/0/17</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -626,12 +626,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>xe-0/0/29</t>
+          <t>xe-0/0/18</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -661,12 +661,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>xe-0/0/30</t>
+          <t>xe-0/0/19</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -696,12 +696,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>xe-0/0/31</t>
+          <t>xe-0/0/20</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -731,12 +731,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>xe-0/0/32</t>
+          <t>xe-0/0/21</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -751,7 +751,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -766,12 +766,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>xe-0/0/33</t>
+          <t>xe-0/0/22</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -801,12 +801,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>xe-0/0/34</t>
+          <t>xe-0/0/23</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -836,12 +836,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>xe-0/0/35</t>
+          <t>xe-0/0/24</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -856,7 +856,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -871,12 +871,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>xe-0/0/36</t>
+          <t>xe-0/0/25</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -906,12 +906,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>xe-0/0/37</t>
+          <t>xe-0/0/26</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -926,7 +926,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -941,12 +941,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>xe-0/0/38</t>
+          <t>xe-0/0/27</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -976,12 +976,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>xe-0/0/39</t>
+          <t>xe-0/0/28</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -996,7 +996,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1011,12 +1011,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>xe-0/0/40</t>
+          <t>xe-0/0/29</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1046,12 +1046,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>xe-0/0/41</t>
+          <t>xe-0/0/30</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1081,12 +1081,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>xe-0/0/42</t>
+          <t>xe-0/0/31</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1116,12 +1116,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>xe-0/0/43</t>
+          <t>xe-0/0/32</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1151,12 +1151,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>xe-0/0/44</t>
+          <t>xe-0/0/33</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1186,12 +1186,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>xe-0/0/45</t>
+          <t>xe-0/0/34</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1221,12 +1221,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>xe-0/0/46</t>
+          <t>xe-0/0/36</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1256,12 +1256,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>xe-0/0/47</t>
+          <t>xe-0/0/37</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1291,12 +1291,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-03-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>xe-0/0/48</t>
+          <t>xe-0/0/38</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1326,12 +1326,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>xe-0/0/0</t>
+          <t>xe-0/0/39</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1361,12 +1361,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>xe-0/0/1</t>
+          <t>xe-0/0/40</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1396,12 +1396,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>xe-0/0/10</t>
+          <t>xe-0/0/41</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1431,12 +1431,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>xe-0/0/11</t>
+          <t>xe-0/0/42</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1451,12 +1451,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>11:0</t>
+          <t>14:0</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1466,12 +1466,12 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>xe-0/0/12</t>
+          <t>xe-0/0/43</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1486,12 +1486,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>11:1</t>
+          <t>14:1</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1501,12 +1501,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>xe-0/0/13</t>
+          <t>xe-0/0/44</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1521,12 +1521,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>12:0</t>
+          <t>15:0</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1536,12 +1536,12 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>xe-0/0/14</t>
+          <t>xe-0/0/45</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1556,12 +1556,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>12:1</t>
+          <t>15:1</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1571,12 +1571,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>xe-0/0/15</t>
+          <t>xe-0/0/46</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1591,12 +1591,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>13:0</t>
+          <t>16:0</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1606,12 +1606,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>xe-0/0/16</t>
+          <t>xe-0/0/47</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1626,12 +1626,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>13:1</t>
+          <t>16:1</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1641,12 +1641,12 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
+          <t>MADRI-MADR-H-01-DAAS</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>xe-0/0/17</t>
+          <t>xe-0/0/48</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1661,12 +1661,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>14:0</t>
+          <t>17:0</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1674,21 +1674,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>xe-0/0/18</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1696,12 +1684,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>14:1</t>
+          <t>17:1</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1709,21 +1697,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>xe-0/0/19</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1731,12 +1707,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>15:0</t>
+          <t>18:0</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1744,21 +1720,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>xe-0/0/2</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1766,12 +1730,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>15:1</t>
+          <t>18:1</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1779,21 +1743,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>xe-0/0/20</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1801,7 +1753,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1814,21 +1766,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>xe-0/0/21</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1836,7 +1776,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1849,21 +1789,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>xe-0/0/22</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1871,7 +1799,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1884,21 +1812,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>xe-0/0/23</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1906,7 +1822,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1919,21 +1835,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>xe-0/0/24</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1941,7 +1845,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1954,21 +1858,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>xe-0/0/25</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1976,7 +1868,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1989,21 +1881,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>xe-0/0/26</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2011,7 +1891,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2024,21 +1904,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>xe-0/0/27</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2046,7 +1914,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2059,21 +1927,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>xe-0/0/28</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2081,7 +1937,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2094,21 +1950,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>xe-0/0/29</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2116,7 +1960,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2129,21 +1973,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>xe-0/0/3</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -2151,7 +1983,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2164,21 +1996,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>xe-0/0/30</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2186,7 +2006,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2199,21 +2019,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>xe-0/0/31</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -2221,7 +2029,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2234,21 +2042,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>xe-0/0/32</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2256,7 +2052,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2269,21 +2065,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>xe-0/0/33</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2291,7 +2075,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2304,21 +2088,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>xe-0/0/34</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2326,7 +2098,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2339,21 +2111,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>xe-0/0/35</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2361,7 +2121,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2374,21 +2134,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>xe-0/0/36</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2396,7 +2144,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2409,21 +2157,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>xe-0/0/37</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2431,7 +2167,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2444,21 +2180,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>xe-0/0/38</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2466,7 +2190,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2479,21 +2203,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>xe-0/0/39</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2501,7 +2213,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2514,21 +2226,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>xe-0/0/4</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2536,7 +2236,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2549,21 +2249,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>xe-0/0/40</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -2571,7 +2259,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2584,21 +2272,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>xe-0/0/41</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2606,7 +2282,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2619,21 +2295,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>xe-0/0/42</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2641,7 +2305,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2654,21 +2318,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>xe-0/0/43</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2676,7 +2328,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2689,21 +2341,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>xe-0/0/44</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2711,7 +2351,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2724,21 +2364,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>xe-0/0/45</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2746,7 +2374,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2759,21 +2387,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>xe-0/0/46</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2781,7 +2397,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2794,21 +2410,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>xe-0/0/47</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2816,7 +2420,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2829,21 +2433,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>xe-0/0/48</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2851,7 +2443,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2864,21 +2456,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>xe-0/0/5</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2886,7 +2466,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2899,21 +2479,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>xe-0/0/6</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2921,7 +2489,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2934,21 +2502,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>xe-0/0/7</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2956,7 +2512,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2969,21 +2525,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>xe-0/0/8</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2991,7 +2535,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3004,21 +2548,9 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-04-DAAS</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>xe-0/0/9</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -3026,7 +2558,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3049,7 +2581,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3072,7 +2604,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3095,7 +2627,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3118,7 +2650,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3141,7 +2673,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3164,7 +2696,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3187,7 +2719,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3210,7 +2742,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3233,7 +2765,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3256,7 +2788,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3279,7 +2811,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3302,7 +2834,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3325,7 +2857,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3348,7 +2880,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3371,7 +2903,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3394,7 +2926,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3417,7 +2949,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3440,7 +2972,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3463,7 +2995,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3486,7 +3018,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3509,7 +3041,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3532,7 +3064,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3555,7 +3087,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3578,7 +3110,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3601,7 +3133,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3624,7 +3156,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3647,7 +3179,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3670,7 +3202,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3693,7 +3225,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3716,7 +3248,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3739,7 +3271,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3762,7 +3294,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3785,7 +3317,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3808,7 +3340,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3831,7 +3363,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3854,7 +3386,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3877,7 +3409,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3900,7 +3432,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3923,7 +3455,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3946,7 +3478,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3969,7 +3501,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3992,7 +3524,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -4015,7 +3547,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4038,7 +3570,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4061,7 +3593,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4084,7 +3616,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -4107,7 +3639,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -4130,7 +3662,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -4153,7 +3685,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4176,7 +3708,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -4199,12 +3731,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>5:0</t>
+          <t>60:0</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -4222,12 +3754,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>5:1</t>
+          <t>60:1</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -4245,12 +3777,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>60:0</t>
+          <t>61:0</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -4268,12 +3800,12 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>60:1</t>
+          <t>61:1</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -4291,12 +3823,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>61:0</t>
+          <t>62:0</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -4314,12 +3846,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>61:1</t>
+          <t>62:1</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -4337,12 +3869,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>62:0</t>
+          <t>63:0</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -4360,12 +3892,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>62:1</t>
+          <t>63:1</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -4383,12 +3915,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>63:0</t>
+          <t>64:0</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -4406,12 +3938,12 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>63:1</t>
+          <t>64:1</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4429,12 +3961,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>64:0</t>
+          <t>65:0</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4452,12 +3984,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>64:1</t>
+          <t>65:1</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4475,12 +4007,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>65:0</t>
+          <t>66:0</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4498,12 +4030,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>65:1</t>
+          <t>66:1</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4521,12 +4053,12 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>66:0</t>
+          <t>67:0</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4544,12 +4076,12 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>66:1</t>
+          <t>67:1</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4567,12 +4099,12 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>67:0</t>
+          <t>68:0</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4590,12 +4122,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>67:1</t>
+          <t>68:1</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4613,12 +4145,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>68:0</t>
+          <t>69:0</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4636,12 +4168,12 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>68:1</t>
+          <t>69:1</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4659,12 +4191,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>69:0</t>
+          <t>6:0</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4682,12 +4214,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>69:1</t>
+          <t>6:1</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4705,12 +4237,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>6:0</t>
+          <t>70:0</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4728,12 +4260,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>6:1</t>
+          <t>70:1</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -4751,12 +4283,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>70:0</t>
+          <t>71:0</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -4774,12 +4306,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>70:1</t>
+          <t>71:1</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -4797,12 +4329,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>71:0</t>
+          <t>72:0</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -4820,12 +4352,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>71:1</t>
+          <t>72:1</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -4843,12 +4375,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>72:0</t>
+          <t>73:0</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -4866,12 +4398,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>72:1</t>
+          <t>73:1</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -4889,12 +4421,12 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>73:0</t>
+          <t>74:0</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -4912,12 +4444,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>73:1</t>
+          <t>74:1</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -4935,12 +4467,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>74:0</t>
+          <t>75:0</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -4958,12 +4490,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>74:1</t>
+          <t>75:1</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -4981,12 +4513,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>75:0</t>
+          <t>76:0</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -5004,12 +4536,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>75:1</t>
+          <t>76:1</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -5027,12 +4559,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>76:0</t>
+          <t>77:0</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -5050,12 +4582,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>76:1</t>
+          <t>77:1</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -5073,12 +4605,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>77:0</t>
+          <t>78:0</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -5096,12 +4628,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>77:1</t>
+          <t>78:1</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -5119,12 +4651,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>78:0</t>
+          <t>79:0</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -5142,12 +4674,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>78:1</t>
+          <t>79:1</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -5165,12 +4697,12 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>79:0</t>
+          <t>80:0</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -5188,12 +4720,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>79:1</t>
+          <t>80:1</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -5211,12 +4743,12 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>7:0</t>
+          <t>81:0</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -5234,12 +4766,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>7:1</t>
+          <t>81:1</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -5257,12 +4789,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>80:0</t>
+          <t>82:0</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -5280,12 +4812,12 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>80:1</t>
+          <t>82:1</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -5303,12 +4835,12 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>81:0</t>
+          <t>83:0</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -5326,12 +4858,12 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>81:1</t>
+          <t>83:1</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -5349,12 +4881,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>82:0</t>
+          <t>84:0</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -5372,12 +4904,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>82:1</t>
+          <t>84:1</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
@@ -5395,12 +4927,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>83:0</t>
+          <t>85:0</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -5418,12 +4950,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>83:1</t>
+          <t>85:1</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -5441,12 +4973,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>84:0</t>
+          <t>86:0</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -5464,12 +4996,12 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>84:1</t>
+          <t>86:1</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -5487,12 +5019,12 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>85:0</t>
+          <t>87:0</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -5510,12 +5042,12 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>85:1</t>
+          <t>87:1</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
@@ -5533,12 +5065,12 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>86:0</t>
+          <t>88:0</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -5556,12 +5088,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>86:1</t>
+          <t>88:1</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -5579,12 +5111,12 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>87:0</t>
+          <t>89:0</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -5602,12 +5134,12 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>87:1</t>
+          <t>89:1</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -5625,12 +5157,12 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>88:0</t>
+          <t>8:0</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -5648,12 +5180,12 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>88:1</t>
+          <t>8:1</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -5671,12 +5203,12 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>89:0</t>
+          <t>90:0</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -5694,12 +5226,12 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>89:1</t>
+          <t>90:1</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -5717,12 +5249,12 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>8:0</t>
+          <t>91:0</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -5740,12 +5272,12 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>8:1</t>
+          <t>91:1</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -5763,12 +5295,12 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>90:0</t>
+          <t>92:0</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
@@ -5786,12 +5318,12 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>90:1</t>
+          <t>92:1</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
@@ -5809,12 +5341,12 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>91:0</t>
+          <t>93:0</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
@@ -5832,12 +5364,12 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>91:1</t>
+          <t>93:1</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
@@ -5855,12 +5387,12 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>92:0</t>
+          <t>94:0</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
@@ -5878,12 +5410,12 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>92:1</t>
+          <t>94:1</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
@@ -5901,12 +5433,12 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>93:0</t>
+          <t>95:0</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -5924,12 +5456,12 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>93:1</t>
+          <t>95:1</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
@@ -5947,12 +5479,12 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>94:0</t>
+          <t>96:0</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
@@ -5970,12 +5502,12 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>94:1</t>
+          <t>96:1</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
@@ -5993,12 +5525,12 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>95:0</t>
+          <t>97:0</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
@@ -6016,12 +5548,12 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>95:1</t>
+          <t>97:1</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
@@ -6039,12 +5571,12 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>96:0</t>
+          <t>98:0</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
@@ -6062,12 +5594,12 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>96:1</t>
+          <t>98:1</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
@@ -6085,12 +5617,12 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>97:0</t>
+          <t>99:0</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
@@ -6108,12 +5640,12 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>97:1</t>
+          <t>99:1</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
@@ -6131,12 +5663,12 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>98:0</t>
+          <t>9:0</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
@@ -6154,12 +5686,12 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>BOGO-GARCE-H-06-COS</t>
+          <t>MADRI-MADR-H-03-COS</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>98:1</t>
+          <t>9:1</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
@@ -6170,98 +5702,6 @@
       <c r="E211" t="inlineStr"/>
       <c r="F211" t="inlineStr"/>
       <c r="G211" t="inlineStr"/>
-    </row>
-    <row r="212">
-      <c r="A212" s="1" t="n">
-        <v>210</v>
-      </c>
-      <c r="B212" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-06-COS</t>
-        </is>
-      </c>
-      <c r="C212" t="inlineStr">
-        <is>
-          <t>99:0</t>
-        </is>
-      </c>
-      <c r="D212" t="inlineStr">
-        <is>
-          <t>unlocked</t>
-        </is>
-      </c>
-      <c r="E212" t="inlineStr"/>
-      <c r="F212" t="inlineStr"/>
-      <c r="G212" t="inlineStr"/>
-    </row>
-    <row r="213">
-      <c r="A213" s="1" t="n">
-        <v>211</v>
-      </c>
-      <c r="B213" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-06-COS</t>
-        </is>
-      </c>
-      <c r="C213" t="inlineStr">
-        <is>
-          <t>99:1</t>
-        </is>
-      </c>
-      <c r="D213" t="inlineStr">
-        <is>
-          <t>unlocked</t>
-        </is>
-      </c>
-      <c r="E213" t="inlineStr"/>
-      <c r="F213" t="inlineStr"/>
-      <c r="G213" t="inlineStr"/>
-    </row>
-    <row r="214">
-      <c r="A214" s="1" t="n">
-        <v>212</v>
-      </c>
-      <c r="B214" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-06-COS</t>
-        </is>
-      </c>
-      <c r="C214" t="inlineStr">
-        <is>
-          <t>9:0</t>
-        </is>
-      </c>
-      <c r="D214" t="inlineStr">
-        <is>
-          <t>unlocked</t>
-        </is>
-      </c>
-      <c r="E214" t="inlineStr"/>
-      <c r="F214" t="inlineStr"/>
-      <c r="G214" t="inlineStr"/>
-    </row>
-    <row r="215">
-      <c r="A215" s="1" t="n">
-        <v>213</v>
-      </c>
-      <c r="B215" t="inlineStr">
-        <is>
-          <t>BOGO-GARCE-H-06-COS</t>
-        </is>
-      </c>
-      <c r="C215" t="inlineStr">
-        <is>
-          <t>9:1</t>
-        </is>
-      </c>
-      <c r="D215" t="inlineStr">
-        <is>
-          <t>unlocked</t>
-        </is>
-      </c>
-      <c r="E215" t="inlineStr"/>
-      <c r="F215" t="inlineStr"/>
-      <c r="G215" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>